<commit_message>
schoolcuts rerun with new costs data
</commit_message>
<xml_diff>
--- a/output/Deprivation.xlsx
+++ b/output/Deprivation.xlsx
@@ -624,106 +624,106 @@
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>3629</v>
+        <v>3612</v>
       </c>
       <c r="C4" s="2">
-        <v>1339673</v>
+        <v>1335967.5</v>
       </c>
       <c r="D4" s="2">
-        <v>1359121.5</v>
+        <v>1355388.5</v>
       </c>
       <c r="E4" s="2">
-        <v>1376324.5</v>
+        <v>1372762.5</v>
       </c>
       <c r="F4" s="2">
-        <v>1391747</v>
+        <v>1388104</v>
       </c>
       <c r="G4" s="2">
-        <v>1407380</v>
+        <v>1403975</v>
       </c>
       <c r="H4" s="2">
-        <v>1419817.5</v>
+        <v>1416371.5</v>
       </c>
       <c r="I4" s="3">
-        <v>8013585968.28858</v>
+        <v>7769340253.07633</v>
       </c>
       <c r="J4" s="3">
-        <v>7944073512.983419</v>
+        <v>7736283000.486543</v>
       </c>
       <c r="K4" s="3">
-        <v>7892243623.889732</v>
+        <v>7702930757.171782</v>
       </c>
       <c r="L4" s="3">
-        <v>7940549140.916016</v>
+        <v>7791774566.322871</v>
       </c>
       <c r="M4" s="3">
-        <v>7765016624.790022</v>
+        <v>7706588459.991132</v>
       </c>
       <c r="N4" s="3">
-        <v>8257858058.30573</v>
+        <v>8203788654.568119</v>
       </c>
       <c r="O4" s="4">
-        <v>0.7305042711490769</v>
+        <v>0.7068106312292359</v>
       </c>
       <c r="P4" s="4">
-        <v>0.7707357398732433</v>
+        <v>0.7397563676633444</v>
       </c>
       <c r="Q4" s="4">
-        <v>0.7547533755855608</v>
+        <v>0.7015503875968992</v>
       </c>
       <c r="R4" s="4">
-        <v>0.8481675392670157</v>
+        <v>0.7630121816168328</v>
       </c>
       <c r="S4" s="4">
-        <v>0.674841554147148</v>
+        <v>0.5586932447397563</v>
       </c>
       <c r="T4" s="5">
-        <v>5981.747761049584</v>
+        <v>5815.515911185213</v>
       </c>
       <c r="U4" s="5">
-        <v>5845.006140351264</v>
+        <v>5707.797432608099</v>
       </c>
       <c r="V4" s="5">
-        <v>5734.289859615034</v>
+        <v>5611.262514216248</v>
       </c>
       <c r="W4" s="5">
-        <v>5705.454469034972</v>
+        <v>5613.24984750629</v>
       </c>
       <c r="X4" s="5">
-        <v>5517.356097706392</v>
+        <v>5489.120860407865</v>
       </c>
       <c r="Y4" s="5">
-        <v>5816.140495736762</v>
+        <v>5792.116443015211</v>
       </c>
       <c r="Z4" s="5">
-        <v>-136.7416206983207</v>
+        <v>-107.7184785771133</v>
       </c>
       <c r="AA4" s="5">
-        <v>-247.45790143455</v>
+        <v>-204.2533969689648</v>
       </c>
       <c r="AB4" s="5">
-        <v>-276.2932920146122</v>
+        <v>-202.2660636789224</v>
       </c>
       <c r="AC4" s="5">
-        <v>-464.3916633431927</v>
+        <v>-326.3950507773479</v>
       </c>
       <c r="AD4" s="5">
-        <v>-165.6072653128222</v>
+        <v>-23.39946817000146</v>
       </c>
       <c r="AE4" s="4">
-        <v>-0.02285981057053588</v>
+        <v>-0.01852260061225763</v>
       </c>
       <c r="AF4" s="4">
-        <v>-0.04136882919836293</v>
+        <v>-0.03512214566830019</v>
       </c>
       <c r="AG4" s="4">
-        <v>-0.04618939197231087</v>
+        <v>-0.03478041617767669</v>
       </c>
       <c r="AH4" s="4">
-        <v>-0.07763477864564927</v>
+        <v>-0.05612486592110932</v>
       </c>
       <c r="AI4" s="4">
-        <v>-0.0276854310693575</v>
+        <v>-0.004023627228840754</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -731,106 +731,106 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>3722</v>
+        <v>3725</v>
       </c>
       <c r="C5" s="2">
-        <v>1319080</v>
+        <v>1319801</v>
       </c>
       <c r="D5" s="2">
-        <v>1340566</v>
+        <v>1341202</v>
       </c>
       <c r="E5" s="2">
-        <v>1362640.5</v>
+        <v>1363421.5</v>
       </c>
       <c r="F5" s="2">
-        <v>1380746</v>
+        <v>1381585.5</v>
       </c>
       <c r="G5" s="2">
-        <v>1396317.5</v>
+        <v>1397192.5</v>
       </c>
       <c r="H5" s="2">
-        <v>1404975</v>
+        <v>1406038.5</v>
       </c>
       <c r="I5" s="3">
-        <v>8266083326.46811</v>
+        <v>8055998951.097355</v>
       </c>
       <c r="J5" s="3">
-        <v>8133936948.141412</v>
+        <v>7959841788.538153</v>
       </c>
       <c r="K5" s="3">
-        <v>8109349069.902622</v>
+        <v>7948783072.3397</v>
       </c>
       <c r="L5" s="3">
-        <v>8179992490.020913</v>
+        <v>8059251459.457801</v>
       </c>
       <c r="M5" s="3">
-        <v>7964494867.926481</v>
+        <v>7939627805.884805</v>
       </c>
       <c r="N5" s="3">
-        <v>8422257974.012113</v>
+        <v>8407253091.374852</v>
       </c>
       <c r="O5" s="4">
-        <v>0.7396560988715745</v>
+        <v>0.7157046979865772</v>
       </c>
       <c r="P5" s="4">
-        <v>0.776732939279957</v>
+        <v>0.7503355704697987</v>
       </c>
       <c r="Q5" s="4">
-        <v>0.7592692101020957</v>
+        <v>0.7130201342281879</v>
       </c>
       <c r="R5" s="4">
-        <v>0.8481998925308973</v>
+        <v>0.7798657718120805</v>
       </c>
       <c r="S5" s="4">
-        <v>0.6792047286405158</v>
+        <v>0.5892617449664429</v>
       </c>
       <c r="T5" s="5">
-        <v>6266.551935036624</v>
+        <v>6103.949725070184</v>
       </c>
       <c r="U5" s="5">
-        <v>6067.539343934884</v>
+        <v>5934.856784092294</v>
       </c>
       <c r="V5" s="5">
-        <v>5951.202147523592</v>
+        <v>5830.026204178018</v>
       </c>
       <c r="W5" s="5">
-        <v>5924.328218239208</v>
+        <v>5833.335294455393</v>
       </c>
       <c r="X5" s="5">
-        <v>5703.928274140001</v>
+        <v>5682.558277320272</v>
       </c>
       <c r="Y5" s="5">
-        <v>5994.59632663365</v>
+        <v>5979.390387514177</v>
       </c>
       <c r="Z5" s="5">
-        <v>-199.0125911017403</v>
+        <v>-169.0929409778901</v>
       </c>
       <c r="AA5" s="5">
-        <v>-315.3497875130315</v>
+        <v>-273.9235208921664</v>
       </c>
       <c r="AB5" s="5">
-        <v>-342.2237167974163</v>
+        <v>-270.6144306147917</v>
       </c>
       <c r="AC5" s="5">
-        <v>-562.6236608966228</v>
+        <v>-421.391447749912</v>
       </c>
       <c r="AD5" s="5">
-        <v>-271.9556084029737</v>
+        <v>-124.5593375560074</v>
       </c>
       <c r="AE5" s="4">
-        <v>-0.03175790979869653</v>
+        <v>-0.02770221718625732</v>
       </c>
       <c r="AF5" s="4">
-        <v>-0.05032269592307914</v>
+        <v>-0.0448764379180755</v>
       </c>
       <c r="AG5" s="4">
-        <v>-0.05461116740835181</v>
+        <v>-0.04433431512440578</v>
       </c>
       <c r="AH5" s="4">
-        <v>-0.08978201517025086</v>
+        <v>-0.0690358647646081</v>
       </c>
       <c r="AI5" s="4">
-        <v>-0.04339796609399427</v>
+        <v>-0.02040635050521733</v>
       </c>
     </row>
     <row r="6" spans="1:35">
@@ -838,106 +838,106 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>3396</v>
+        <v>3387</v>
       </c>
       <c r="C6" s="2">
-        <v>1285781</v>
+        <v>1279438.5</v>
       </c>
       <c r="D6" s="2">
-        <v>1306157.5</v>
+        <v>1299649</v>
       </c>
       <c r="E6" s="2">
-        <v>1325119</v>
+        <v>1318799.5</v>
       </c>
       <c r="F6" s="2">
-        <v>1341808.5</v>
+        <v>1335437</v>
       </c>
       <c r="G6" s="2">
-        <v>1353453</v>
+        <v>1346978.5</v>
       </c>
       <c r="H6" s="2">
-        <v>1357124.5</v>
+        <v>1350445.5</v>
       </c>
       <c r="I6" s="3">
-        <v>8440718759.991749</v>
+        <v>8173875948.201067</v>
       </c>
       <c r="J6" s="3">
-        <v>8217516745.420856</v>
+        <v>7986558687.475271</v>
       </c>
       <c r="K6" s="3">
-        <v>8178343192.127323</v>
+        <v>7970616591.868944</v>
       </c>
       <c r="L6" s="3">
-        <v>8218538937.166388</v>
+        <v>8046481424.204811</v>
       </c>
       <c r="M6" s="3">
-        <v>8017918510.181868</v>
+        <v>7949054741.263597</v>
       </c>
       <c r="N6" s="3">
-        <v>8411837585.307708</v>
+        <v>8337419851.870849</v>
       </c>
       <c r="O6" s="4">
-        <v>0.7712014134275619</v>
+        <v>0.7440212577502214</v>
       </c>
       <c r="P6" s="4">
-        <v>0.7924028268551236</v>
+        <v>0.7676409802184825</v>
       </c>
       <c r="Q6" s="4">
-        <v>0.7788574793875147</v>
+        <v>0.734573368762917</v>
       </c>
       <c r="R6" s="4">
-        <v>0.8486454652532391</v>
+        <v>0.7894892235016239</v>
       </c>
       <c r="S6" s="4">
-        <v>0.7229093050647821</v>
+        <v>0.6259226454089164</v>
       </c>
       <c r="T6" s="5">
-        <v>6564.662846932525</v>
+        <v>6388.643102580599</v>
       </c>
       <c r="U6" s="5">
-        <v>6291.367423469876</v>
+        <v>6145.1658774602</v>
       </c>
       <c r="V6" s="5">
-        <v>6171.780188894222</v>
+        <v>6043.842594624083</v>
       </c>
       <c r="W6" s="5">
-        <v>6124.971586605978</v>
+        <v>6025.354564988697</v>
       </c>
       <c r="X6" s="5">
-        <v>5924.046501933844</v>
+        <v>5901.396897770526</v>
       </c>
       <c r="Y6" s="5">
-        <v>6198.279955381918</v>
+        <v>6173.829193307578</v>
       </c>
       <c r="Z6" s="5">
-        <v>-273.2954234626486</v>
+        <v>-243.4772251203985</v>
       </c>
       <c r="AA6" s="5">
-        <v>-392.8826580383029</v>
+        <v>-344.8005079565155</v>
       </c>
       <c r="AB6" s="5">
-        <v>-439.6912603265473</v>
+        <v>-363.2885375919013</v>
       </c>
       <c r="AC6" s="5">
-        <v>-640.6163449986807</v>
+        <v>-487.2462048100724</v>
       </c>
       <c r="AD6" s="5">
-        <v>-366.3828915506074</v>
+        <v>-214.8139092730207</v>
       </c>
       <c r="AE6" s="4">
-        <v>-0.04163129620439709</v>
+        <v>-0.03811094487686273</v>
       </c>
       <c r="AF6" s="4">
-        <v>-0.05984810906502003</v>
+        <v>-0.05397085146566383</v>
       </c>
       <c r="AG6" s="4">
-        <v>-0.06697849845129555</v>
+        <v>-0.05686474134783903</v>
       </c>
       <c r="AH6" s="4">
-        <v>-0.09758556683501607</v>
+        <v>-0.07626755744318481</v>
       </c>
       <c r="AI6" s="4">
-        <v>-0.05581137982155582</v>
+        <v>-0.03362434022746552</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -945,106 +945,106 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>3510</v>
+        <v>3497</v>
       </c>
       <c r="C7" s="2">
-        <v>1339104</v>
+        <v>1337326</v>
       </c>
       <c r="D7" s="2">
-        <v>1361777</v>
+        <v>1359893</v>
       </c>
       <c r="E7" s="2">
-        <v>1376204.5</v>
+        <v>1374499.5</v>
       </c>
       <c r="F7" s="2">
-        <v>1391933</v>
+        <v>1390836</v>
       </c>
       <c r="G7" s="2">
-        <v>1402944.5</v>
+        <v>1402092.5</v>
       </c>
       <c r="H7" s="2">
-        <v>1402877.5</v>
+        <v>1402158.5</v>
       </c>
       <c r="I7" s="3">
-        <v>9546611442.233463</v>
+        <v>9285119972.49873</v>
       </c>
       <c r="J7" s="3">
-        <v>9264964293.876554</v>
+        <v>9042625665.008123</v>
       </c>
       <c r="K7" s="3">
-        <v>9212097169.518721</v>
+        <v>9012994870.710146</v>
       </c>
       <c r="L7" s="3">
-        <v>9219176496.615822</v>
+        <v>9065934735.583771</v>
       </c>
       <c r="M7" s="3">
-        <v>8976921172.70557</v>
+        <v>8937067093.97122</v>
       </c>
       <c r="N7" s="3">
-        <v>9344578890.509977</v>
+        <v>9306560478.133169</v>
       </c>
       <c r="O7" s="4">
-        <v>0.7678062678062678</v>
+        <v>0.7489276522733772</v>
       </c>
       <c r="P7" s="4">
-        <v>0.7783475783475784</v>
+        <v>0.7577923934801258</v>
       </c>
       <c r="Q7" s="4">
-        <v>0.7897435897435897</v>
+        <v>0.7500714898484415</v>
       </c>
       <c r="R7" s="4">
-        <v>0.8623931623931624</v>
+        <v>0.8049756934515299</v>
       </c>
       <c r="S7" s="4">
-        <v>0.7279202279202279</v>
+        <v>0.6454103517300543</v>
       </c>
       <c r="T7" s="5">
-        <v>7129.103820340663</v>
+        <v>6943.049019086393</v>
       </c>
       <c r="U7" s="5">
-        <v>6803.584062498158</v>
+        <v>6649.512619748851</v>
       </c>
       <c r="V7" s="5">
-        <v>6693.843225711528</v>
+        <v>6557.292214882687</v>
       </c>
       <c r="W7" s="5">
-        <v>6623.290414564366</v>
+        <v>6518.334825661524</v>
       </c>
       <c r="X7" s="5">
-        <v>6398.628864296179</v>
+        <v>6374.092361218122</v>
       </c>
       <c r="Y7" s="5">
-        <v>6661.008456198048</v>
+        <v>6637.30988909825</v>
       </c>
       <c r="Z7" s="5">
-        <v>-325.519757842505</v>
+        <v>-293.5363993375422</v>
       </c>
       <c r="AA7" s="5">
-        <v>-435.2605946291351</v>
+        <v>-385.7568042037055</v>
       </c>
       <c r="AB7" s="5">
-        <v>-505.8134057762973</v>
+        <v>-424.7141934248693</v>
       </c>
       <c r="AC7" s="5">
-        <v>-730.4749560444843</v>
+        <v>-568.9566578682707</v>
       </c>
       <c r="AD7" s="5">
-        <v>-468.0953641426149</v>
+        <v>-305.7391299881428</v>
       </c>
       <c r="AE7" s="4">
-        <v>-0.04566068415411995</v>
+        <v>-0.04227773684596103</v>
       </c>
       <c r="AF7" s="4">
-        <v>-0.06105404067580777</v>
+        <v>-0.05556014413023191</v>
       </c>
       <c r="AG7" s="4">
-        <v>-0.07095048950376026</v>
+        <v>-0.06117113565773957</v>
       </c>
       <c r="AH7" s="4">
-        <v>-0.1024637842922561</v>
+        <v>-0.08194622511006511</v>
       </c>
       <c r="AI7" s="4">
-        <v>-0.06565977659170164</v>
+        <v>-0.04403528322321626</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -1052,106 +1052,106 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>3360</v>
+        <v>3353</v>
       </c>
       <c r="C8" s="2">
-        <v>1230284</v>
+        <v>1227172</v>
       </c>
       <c r="D8" s="2">
-        <v>1247477</v>
+        <v>1244346.5</v>
       </c>
       <c r="E8" s="2">
-        <v>1256720</v>
+        <v>1253977</v>
       </c>
       <c r="F8" s="2">
-        <v>1265505</v>
+        <v>1262701.5</v>
       </c>
       <c r="G8" s="2">
-        <v>1268607</v>
+        <v>1265795</v>
       </c>
       <c r="H8" s="2">
-        <v>1261447.5</v>
+        <v>1258617</v>
       </c>
       <c r="I8" s="3">
-        <v>9566605338.489342</v>
+        <v>9274138473.364799</v>
       </c>
       <c r="J8" s="3">
-        <v>9221797001.952103</v>
+        <v>8979521925.002832</v>
       </c>
       <c r="K8" s="3">
-        <v>9147310915.672699</v>
+        <v>8921212200.572533</v>
       </c>
       <c r="L8" s="3">
-        <v>9101160881.456114</v>
+        <v>8927661349.425362</v>
       </c>
       <c r="M8" s="3">
-        <v>8831886296.392302</v>
+        <v>8769093263.025267</v>
       </c>
       <c r="N8" s="3">
-        <v>9130935208.112324</v>
+        <v>9063870295.610519</v>
       </c>
       <c r="O8" s="4">
-        <v>0.7690476190476191</v>
+        <v>0.7482851178049508</v>
       </c>
       <c r="P8" s="4">
-        <v>0.7729166666666667</v>
+        <v>0.7488815985684462</v>
       </c>
       <c r="Q8" s="4">
-        <v>0.7827380952380952</v>
+        <v>0.7363555025350432</v>
       </c>
       <c r="R8" s="4">
-        <v>0.8517857142857143</v>
+        <v>0.7894422904861318</v>
       </c>
       <c r="S8" s="4">
-        <v>0.7282738095238095</v>
+        <v>0.6394273784670444</v>
       </c>
       <c r="T8" s="5">
-        <v>7775.932498910285</v>
+        <v>7557.325683249617</v>
       </c>
       <c r="U8" s="5">
-        <v>7392.358337630355</v>
+        <v>7216.255219107245</v>
       </c>
       <c r="V8" s="5">
-        <v>7278.718342727655</v>
+        <v>7114.334792880996</v>
       </c>
       <c r="W8" s="5">
-        <v>7191.722578303613</v>
+        <v>7070.286484513847</v>
       </c>
       <c r="X8" s="5">
-        <v>6961.877316136756</v>
+        <v>6927.735741589488</v>
       </c>
       <c r="Y8" s="5">
-        <v>7238.458364785157</v>
+        <v>7201.452304879498</v>
       </c>
       <c r="Z8" s="5">
-        <v>-383.5741612799302</v>
+        <v>-341.0704641423727</v>
       </c>
       <c r="AA8" s="5">
-        <v>-497.2141561826302</v>
+        <v>-442.990890368621</v>
       </c>
       <c r="AB8" s="5">
-        <v>-584.2099206066723</v>
+        <v>-487.0391987357698</v>
       </c>
       <c r="AC8" s="5">
-        <v>-814.0551827735289</v>
+        <v>-629.5899416601287</v>
       </c>
       <c r="AD8" s="5">
-        <v>-537.4741341251283</v>
+        <v>-355.8733783701191</v>
       </c>
       <c r="AE8" s="4">
-        <v>-0.04932838104416215</v>
+        <v>-0.04513110568971979</v>
       </c>
       <c r="AF8" s="4">
-        <v>-0.06394270478200648</v>
+        <v>-0.05861741427268186</v>
       </c>
       <c r="AG8" s="4">
-        <v>-0.0751305288064863</v>
+        <v>-0.06444597191507362</v>
       </c>
       <c r="AH8" s="4">
-        <v>-0.1046890752829465</v>
+        <v>-0.0833085628498953</v>
       </c>
       <c r="AI8" s="4">
-        <v>-0.06912021602559559</v>
+        <v>-0.04708985602656934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>